<commit_message>
modifier le fichier dataops
</commit_message>
<xml_diff>
--- a/dataops.xlsx
+++ b/dataops.xlsx
@@ -1,26 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C71885B0-8900-4DA5-8D8D-1BECAF8BE101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>prenom</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>sexe</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,7 +82,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,7 +111,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +123,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -144,6 +170,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +222,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +390,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>